<commit_message>
base para detalle de operacion
</commit_message>
<xml_diff>
--- a/assets/plantilla_detalle_operaciones.xlsx
+++ b/assets/plantilla_detalle_operaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Moggia\pdfs-to-excel\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5665DC6A-E244-4D7A-A0D3-687D9333F489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCE57F82-08E8-44E0-BF6D-DA7810D8A2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detalle Operaciones" sheetId="1" r:id="rId1"/>
@@ -287,25 +287,25 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1343025</xdr:colOff>
+      <xdr:colOff>1038225</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19BD1FE4-3150-4ACD-73FE-E1432031FC4A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -327,8 +327,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="6048375" cy="866775"/>
+          <a:off x="38100" y="0"/>
+          <a:ext cx="5667375" cy="933450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -625,22 +625,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="5" width="16" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -763,8 +759,8 @@
     <mergeCell ref="A9:E9"/>
   </mergeCells>
   <printOptions gridLines="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="99" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>